<commit_message>
Updated SDY after video repair
</commit_message>
<xml_diff>
--- a/data/uac_network.xlsx
+++ b/data/uac_network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B01CC06-6909-2547-ACE5-6D18F21EE6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4276FB9F-5EF1-8947-BC7B-1E122801BC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1820" windowWidth="27240" windowHeight="16440" xr2:uid="{C276EF8E-8567-464E-98DC-2A8DA10DDBB6}"/>
+    <workbookView xWindow="-49420" yWindow="-19060" windowWidth="48480" windowHeight="28580" xr2:uid="{C276EF8E-8567-464E-98DC-2A8DA10DDBB6}"/>
   </bookViews>
   <sheets>
     <sheet name="network" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">network!$A$1:$L$43</definedName>
     <definedName name="taxrate">'[1]mixer costs'!$I$2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="256">
   <si>
     <t>NSCU-A004</t>
   </si>
@@ -813,6 +813,39 @@
   </si>
   <si>
     <t>AssetTag</t>
+  </si>
+  <si>
+    <t>2308-0003</t>
+  </si>
+  <si>
+    <t>Youth Projector</t>
+  </si>
+  <si>
+    <t>Sony VPL-EW575</t>
+  </si>
+  <si>
+    <t>1c:e1:92:6d:1f:0B</t>
+  </si>
+  <si>
+    <t>192.168.0.117</t>
+  </si>
+  <si>
+    <t>youthswitch</t>
+  </si>
+  <si>
+    <t>IP is dynamic … maybe changed to reserved.</t>
+  </si>
+  <si>
+    <t>20:a5:cb:ce:4e:b8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wifi MAC 20:A5:CB:CC:90:2C </t>
+  </si>
+  <si>
+    <t>192.168.0.206</t>
+  </si>
+  <si>
+    <t>http://192.168.0.206:1880/ui</t>
   </si>
 </sst>
 </file>
@@ -971,7 +1004,7 @@
       <sheetName val="PeopleSkill"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="2">
           <cell r="I2">
@@ -979,22 +1012,22 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1297,11 +1330,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC7A309-0B6A-4549-9590-6CFCF97D2DB0}">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2943,8 +2976,47 @@
       <c r="F50" t="s">
         <v>1</v>
       </c>
+      <c r="G50" t="s">
+        <v>252</v>
+      </c>
+      <c r="I50" t="s">
+        <v>254</v>
+      </c>
+      <c r="J50" s="6" t="s">
+        <v>255</v>
+      </c>
       <c r="K50" t="s">
         <v>0</v>
+      </c>
+      <c r="L50" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E51" t="s">
+        <v>246</v>
+      </c>
+      <c r="F51" t="s">
+        <v>247</v>
+      </c>
+      <c r="G51" t="s">
+        <v>248</v>
+      </c>
+      <c r="I51" t="s">
+        <v>249</v>
+      </c>
+      <c r="J51" s="6" t="str">
+        <f>CONCATENATE("http://", I51)</f>
+        <v>http://192.168.0.117</v>
+      </c>
+      <c r="K51" t="s">
+        <v>250</v>
+      </c>
+      <c r="L51" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -2961,9 +3033,11 @@
     <hyperlink ref="J26" r:id="rId10" display="http://192.169.0.112" xr:uid="{AB470B5E-F9C0-024E-9108-70C9861C5095}"/>
     <hyperlink ref="J20" r:id="rId11" display="http://192.169.0.112" xr:uid="{2FA0DCAE-2864-024C-9351-79F3CBFD408D}"/>
     <hyperlink ref="J21" r:id="rId12" display="http://192.169.0.112" xr:uid="{0E717F48-1348-0440-9A96-15E3AB13C8AE}"/>
+    <hyperlink ref="J51" r:id="rId13" display="http://192.169.0.112" xr:uid="{B7709A6B-F68E-6F45-9F1A-5CCF46F3BFD7}"/>
+    <hyperlink ref="J50" r:id="rId14" xr:uid="{1E401A50-9F56-E445-A449-745E383A107C}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId13"/>
+  <legacyDrawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cleared TODOs and corrections
</commit_message>
<xml_diff>
--- a/data/uac_network.xlsx
+++ b/data/uac_network.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4276FB9F-5EF1-8947-BC7B-1E122801BC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A606745C-5897-8B48-B149-FB491B9E7E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-49420" yWindow="-19060" windowWidth="48480" windowHeight="28580" xr2:uid="{C276EF8E-8567-464E-98DC-2A8DA10DDBB6}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="257">
   <si>
     <t>NSCU-A004</t>
   </si>
@@ -846,6 +846,9 @@
   </si>
   <si>
     <t>http://192.168.0.206:1880/ui</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -1332,17 +1335,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC7A309-0B6A-4549-9590-6CFCF97D2DB0}">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
     <col min="5" max="5" width="22.6640625" customWidth="1"/>
     <col min="6" max="6" width="25.33203125" customWidth="1"/>
     <col min="7" max="7" width="20.33203125" customWidth="1"/>
@@ -2841,6 +2844,9 @@
       <c r="A44" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="B44" t="s">
+        <v>256</v>
+      </c>
       <c r="E44" t="s">
         <v>34</v>
       </c>
@@ -2861,6 +2867,9 @@
       <c r="A45" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="B45" t="s">
+        <v>108</v>
+      </c>
       <c r="E45" t="s">
         <v>29</v>
       </c>
@@ -2881,6 +2890,9 @@
       <c r="A46" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="B46" t="s">
+        <v>108</v>
+      </c>
       <c r="E46" t="s">
         <v>24</v>
       </c>
@@ -2901,6 +2913,9 @@
       <c r="A47" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="B47" t="s">
+        <v>108</v>
+      </c>
       <c r="E47" t="s">
         <v>20</v>
       </c>
@@ -2921,6 +2936,9 @@
       <c r="A48" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B48" t="s">
+        <v>108</v>
+      </c>
       <c r="E48" t="s">
         <v>16</v>
       </c>
@@ -2944,6 +2962,9 @@
       <c r="A49" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B49" t="s">
+        <v>75</v>
+      </c>
       <c r="E49" t="s">
         <v>10</v>
       </c>
@@ -2970,6 +2991,9 @@
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B50" t="s">
+        <v>108</v>
+      </c>
       <c r="E50" t="s">
         <v>2</v>
       </c>
@@ -2995,6 +3019,9 @@
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>245</v>
+      </c>
+      <c r="B51" t="s">
+        <v>108</v>
       </c>
       <c r="E51" t="s">
         <v>246</v>

</xml_diff>

<commit_message>
data updates pre avli install
</commit_message>
<xml_diff>
--- a/data/uac_network.xlsx
+++ b/data/uac_network.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donert/Documents/UACTech/SystemDocumentation/github/uactechdoc/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B0FAC82-FD3B-C647-B40D-B09CB9255E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4D1455-7781-DD45-BCBF-3D10F4CEC56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{C276EF8E-8567-464E-98DC-2A8DA10DDBB6}"/>
   </bookViews>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="266">
   <si>
     <t>NSCU-A004</t>
   </si>
@@ -846,13 +846,43 @@
   </si>
   <si>
     <t>192.168.0.208</t>
+  </si>
+  <si>
+    <t>192.168.0.103</t>
+  </si>
+  <si>
+    <t>ZVIU-G001</t>
+  </si>
+  <si>
+    <t>1C-69-7A-66-87-69</t>
+  </si>
+  <si>
+    <t>2405-1307</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Door Access Controller</t>
+  </si>
+  <si>
+    <t>Verkada Door Control</t>
+  </si>
+  <si>
+    <t>E0:A7:00:3F:55:77</t>
+  </si>
+  <si>
+    <t>192.168.0.239</t>
+  </si>
+  <si>
+    <t>amp room</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -916,6 +946,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -931,7 +967,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -939,12 +975,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -959,6 +1006,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1034,9 +1083,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1074,7 +1123,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1180,7 +1229,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1322,7 +1371,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1330,11 +1379,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC7A309-0B6A-4549-9590-6CFCF97D2DB0}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L51" sqref="L51"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2900,7 +2949,7 @@
         <v>22</v>
       </c>
       <c r="I46" t="s">
-        <v>13</v>
+        <v>256</v>
       </c>
       <c r="K46" t="s">
         <v>0</v>
@@ -3038,6 +3087,40 @@
       </c>
       <c r="K51" t="s">
         <v>249</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B52" t="s">
+        <v>108</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="B53" t="s">
+        <v>260</v>
+      </c>
+      <c r="E53" t="s">
+        <v>261</v>
+      </c>
+      <c r="F53" t="s">
+        <v>262</v>
+      </c>
+      <c r="G53" t="s">
+        <v>263</v>
+      </c>
+      <c r="I53" t="s">
+        <v>264</v>
+      </c>
+      <c r="K53" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>